<commit_message>
carga de imagenes para certificado y archivo xlsx de ejemplo para la situacion planteada
</commit_message>
<xml_diff>
--- a/public/ejemplo-carga.xlsx
+++ b/public/ejemplo-carga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyeccionSocial\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31864953-B1BC-4695-BCD5-B700BD64137E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D7AD4D-6148-4225-975D-AD3E414660E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89225295-1B4F-4398-8825-9DC914083096}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>Presencial</t>
   </si>
   <si>
-    <t>Certifica que</t>
-  </si>
-  <si>
     <t>Seguridad digital: Virus informático</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>consecutivo</t>
   </si>
   <si>
-    <t>subtitulo</t>
-  </si>
-  <si>
     <t>nombre_producto</t>
   </si>
   <si>
@@ -204,13 +198,34 @@
   </si>
   <si>
     <t>00004</t>
+  </si>
+  <si>
+    <t>firma_aliado</t>
+  </si>
+  <si>
+    <t>logo_aliado</t>
+  </si>
+  <si>
+    <t>00005</t>
+  </si>
+  <si>
+    <t>Servicio al cliente</t>
+  </si>
+  <si>
+    <t>johan camilo triana avendaño</t>
+  </si>
+  <si>
+    <t>2023/06/20</t>
+  </si>
+  <si>
+    <t>johan_trianaa@cun.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +244,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,118 +596,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01DE92E-CF94-4257-937D-796487E67E3B}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K2" sqref="K2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" t="s">
-        <v>37</v>
-      </c>
-      <c r="W1" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -694,202 +718,299 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2">
+        <v>1022348425</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
-        <v>1022348425</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I2" s="2">
         <v>20</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2">
+        <v>3057186840</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="2">
-        <v>3057186840</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2">
+        <v>5</v>
+      </c>
+      <c r="T2" s="2">
+        <v>5</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="2">
-        <v>5</v>
-      </c>
-      <c r="S2" s="2">
-        <v>5</v>
-      </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="AF2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG2" s="2">
+        <v>12</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH2" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1024572543</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
-        <v>1024572543</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>5</v>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="2">
         <v>20</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2">
+        <v>3057186840</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="2">
+      <c r="Q3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5</v>
+      </c>
+      <c r="T3" s="2">
+        <v>5</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1073230346</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4">
         <v>3057186840</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="O4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S4" s="2">
+        <v>5</v>
+      </c>
+      <c r="T4" s="2">
+        <v>5</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="2">
-        <v>5</v>
-      </c>
-      <c r="S3" s="2">
-        <v>5</v>
-      </c>
-      <c r="T3" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="W4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG3" s="2">
+      <c r="AF4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH4" s="2">
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{2EE58459-9813-4A9D-90E8-A51214453740}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{29F476FD-4174-4AA6-8E0C-ABD996E12364}"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{2EE58459-9813-4A9D-90E8-A51214453740}"/>
+    <hyperlink ref="O3" r:id="rId2" xr:uid="{29F476FD-4174-4AA6-8E0C-ABD996E12364}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>

</xml_diff>

<commit_message>
Ajueste envio de Correos
</commit_message>
<xml_diff>
--- a/public/ejemplo-carga.xlsx
+++ b/public/ejemplo-carga.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyeccionSocial\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D7AD4D-6148-4225-975D-AD3E414660E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BF0BC0-81C3-4DC2-AD9F-0C7939AF9AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89225295-1B4F-4398-8825-9DC914083096}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>Presencial</t>
   </si>
   <si>
-    <t>Seguridad digital: Virus informático</t>
-  </si>
-  <si>
     <t>Janluy Leonard Moreno Coronado</t>
   </si>
   <si>
@@ -188,37 +185,37 @@
     <t>informacion_educativa</t>
   </si>
   <si>
-    <t>janluy_moreno@cun.edu.co</t>
-  </si>
-  <si>
     <t>nelson_cardenas@cun.edu.co</t>
   </si>
   <si>
+    <t>firma_aliado</t>
+  </si>
+  <si>
+    <t>logo_aliado</t>
+  </si>
+  <si>
+    <t>johan camilo triana avendaño</t>
+  </si>
+  <si>
+    <t>2023/06/20</t>
+  </si>
+  <si>
+    <t>johan_trianaa@cun.edu.co</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>00002</t>
+  </si>
+  <si>
     <t>00003</t>
   </si>
   <si>
-    <t>00004</t>
-  </si>
-  <si>
-    <t>firma_aliado</t>
-  </si>
-  <si>
-    <t>logo_aliado</t>
-  </si>
-  <si>
-    <t>00005</t>
-  </si>
-  <si>
-    <t>Servicio al cliente</t>
-  </si>
-  <si>
-    <t>johan camilo triana avendaño</t>
-  </si>
-  <si>
-    <t>2023/06/20</t>
-  </si>
-  <si>
-    <t>johan_trianaa@cun.edu.co</t>
+    <t>ortografia</t>
+  </si>
+  <si>
+    <t>janluy.moreno@cun.edu.co</t>
   </si>
 </sst>
 </file>
@@ -599,165 +596,169 @@
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>44</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="E2" s="2">
         <v>1022348425</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N2" s="2">
         <v>3057186840</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="S2" s="2">
         <v>5</v>
@@ -766,43 +767,43 @@
         <v>5</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="AF2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AH2" s="2">
         <v>100</v>
@@ -810,54 +811,54 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
         <v>1024572543</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="I3" s="2">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N3" s="2">
         <v>3057186840</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="S3" s="2">
         <v>5</v>
@@ -866,43 +867,43 @@
         <v>5</v>
       </c>
       <c r="U3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AE3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="AF3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AH3" s="2">
         <v>100</v>
@@ -910,52 +911,52 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
         <v>57</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>1073230346</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I4">
         <v>8</v>
       </c>
       <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
         <v>5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
       </c>
       <c r="N4">
         <v>3057186840</v>
       </c>
       <c r="O4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="S4" s="2">
         <v>5</v>
@@ -964,43 +965,43 @@
         <v>5</v>
       </c>
       <c r="U4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Z4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AE4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="AF4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AH4" s="2">
         <v>100</v>

</xml_diff>